<commit_message>
mapping audio file is almost completed
</commit_message>
<xml_diff>
--- a/jpr_version2/configurationFile - 복사본.xlsx
+++ b/jpr_version2/configurationFile - 복사본.xlsx
@@ -1,21 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\khw\Desktop\hyunwoo\git\JPR\jpr_version2\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="24">
   <si>
     <t>박스</t>
   </si>
@@ -81,28 +85,48 @@
   </si>
   <si>
     <t>배경만</t>
+  </si>
+  <si>
+    <t>택배발송</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기타</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <name val="Calibri"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -115,15 +139,25 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -411,239 +445,155 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="n">
-        <v>13</v>
-      </c>
-      <c r="B1" t="n">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1">
+        <v>11</v>
+      </c>
+      <c r="B1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" t="s"/>
-      <c r="I2" t="s"/>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>10</v>
       </c>
-      <c r="H3" t="s"/>
-      <c r="I3" t="s"/>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
       </c>
       <c r="D4" t="s">
         <v>13</v>
       </c>
       <c r="E4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" t="s">
         <v>12</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>14</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>15</v>
       </c>
-      <c r="H4" t="s"/>
-      <c r="I4" t="s"/>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
         <v>16</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>17</v>
-      </c>
-      <c r="C5" t="s">
-        <v>9</v>
       </c>
       <c r="D5" t="s">
         <v>9</v>
       </c>
-      <c r="E5" t="s"/>
-      <c r="F5" t="s">
+      <c r="E5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" t="s">
         <v>18</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>19</v>
       </c>
-      <c r="H5" t="s"/>
-      <c r="I5" t="s"/>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
         <v>20</v>
       </c>
-      <c r="B6" t="s"/>
-      <c r="C6" t="s"/>
-      <c r="D6" t="s"/>
-      <c r="E6" t="s"/>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>5</v>
       </c>
-      <c r="G6" t="s">
-        <v>8</v>
-      </c>
-      <c r="H6" t="s"/>
-      <c r="I6" t="s"/>
-    </row>
-    <row r="7">
-      <c r="A7" t="s"/>
-      <c r="B7" t="s"/>
-      <c r="C7" t="s"/>
-      <c r="D7" t="s"/>
-      <c r="E7" t="s"/>
-      <c r="F7" t="s">
+      <c r="H6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G7" t="s">
         <v>21</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>12</v>
       </c>
-      <c r="H7" t="s"/>
-      <c r="I7" t="s"/>
-    </row>
-    <row r="8">
-      <c r="A8" t="s"/>
-      <c r="B8" t="s"/>
-      <c r="C8" t="s"/>
-      <c r="D8" t="s"/>
-      <c r="E8" t="s"/>
-      <c r="F8" t="s">
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G8" t="s">
         <v>13</v>
       </c>
-      <c r="G8" t="s"/>
-      <c r="H8" t="s"/>
-      <c r="I8" t="s"/>
-    </row>
-    <row r="9">
-      <c r="A9" t="s"/>
-      <c r="B9" t="s"/>
-      <c r="C9" t="s"/>
-      <c r="D9" t="s"/>
-      <c r="E9" t="s"/>
-      <c r="F9" t="s">
-        <v>8</v>
-      </c>
-      <c r="G9" t="s"/>
-      <c r="H9" t="s"/>
-      <c r="I9" t="s"/>
-    </row>
-    <row r="10">
-      <c r="A10" t="s"/>
-      <c r="B10" t="s"/>
-      <c r="C10" t="s"/>
-      <c r="D10" t="s"/>
-      <c r="E10" t="s"/>
-      <c r="F10" t="s">
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G10" t="s">
         <v>12</v>
       </c>
-      <c r="G10" t="s"/>
-      <c r="H10" t="s"/>
-      <c r="I10" t="s"/>
-    </row>
-    <row r="11">
-      <c r="A11" t="s"/>
-      <c r="B11" t="s"/>
-      <c r="C11" t="s"/>
-      <c r="D11" t="s"/>
-      <c r="E11" t="s"/>
-      <c r="F11" t="s"/>
-      <c r="G11" t="s"/>
-      <c r="H11" t="s"/>
-      <c r="I11" t="s"/>
-    </row>
-    <row r="12">
-      <c r="A12" t="s"/>
-      <c r="B12" t="s"/>
-      <c r="C12" t="s"/>
-      <c r="D12" t="s"/>
-      <c r="E12" t="s"/>
-      <c r="F12" t="s"/>
-      <c r="G12" t="s"/>
-      <c r="H12" t="s"/>
-      <c r="I12" t="s"/>
-    </row>
-    <row r="13">
-      <c r="A13" t="s"/>
-      <c r="B13" t="s"/>
-      <c r="C13" t="s"/>
-      <c r="D13" t="s"/>
-      <c r="E13" t="s"/>
-      <c r="F13" t="s"/>
-      <c r="G13" t="s"/>
-      <c r="H13" t="s"/>
-      <c r="I13" t="s"/>
-    </row>
-    <row r="14">
-      <c r="A14" t="s"/>
-      <c r="B14" t="s"/>
-      <c r="C14" t="s"/>
-      <c r="D14" t="s"/>
-      <c r="E14" t="s"/>
-      <c r="F14" t="s"/>
-      <c r="G14" t="s"/>
-      <c r="H14" t="s"/>
-      <c r="I14" t="s"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
user configuration and audio - file mapping was done
</commit_message>
<xml_diff>
--- a/jpr_version2/configurationFile - 복사본.xlsx
+++ b/jpr_version2/configurationFile - 복사본.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\khw\Desktop\hyunwoo\git\JPR\jpr_version2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hyunwoo\Desktop\GIT\JPR\jpr_version2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="22">
   <si>
     <t>박스</t>
   </si>
@@ -85,20 +85,12 @@
   </si>
   <si>
     <t>배경만</t>
-  </si>
-  <si>
-    <t>택배발송</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>기타</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -446,54 +438,51 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
@@ -505,89 +494,80 @@
         <v>8</v>
       </c>
       <c r="F3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
         <v>13</v>
       </c>
       <c r="E4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F8" t="s">
         <v>13</v>
       </c>
-      <c r="F4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H6" t="s">
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="G7" t="s">
-        <v>21</v>
-      </c>
-      <c r="H7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="G8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="G9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="G10" t="s">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F10" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>